<commit_message>
updated hard coded values to system properties
</commit_message>
<xml_diff>
--- a/src/main/resources/Book2.xlsx
+++ b/src/main/resources/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adekoyaadeeko/Documents/workspace-spring-tool-suite-4-4.8.1.RELEASE/Swapi-API-Test/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adekoyaadeeko/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{013660FD-BDB8-C746-9915-6A36F0A88A37}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E68B225D-9E8E-5E4B-91CC-F50520426825}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="21140" windowWidth="19560" xWindow="16540" xr2:uid="{1381A3F1-CEB9-4147-B3CF-D43019EFF928}" yWindow="460"/>
+    <workbookView windowHeight="15000" windowWidth="24780" xWindow="740" xr2:uid="{5C360173-2169-794E-88D0-30B3790E3168}" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -637,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D1082A-0260-6F48-9C1A-515F30C6D40F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B043E366-2672-A440-9697-917352D64206}">
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>